<commit_message>
fixed templates a bit
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_РХБЗ.xlsx
+++ b/templates/ведомость_курсанты_РХБЗ.xlsx
@@ -12,19 +12,19 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985"/>
   </bookViews>
   <sheets>
-    <sheet name="ОВУ" sheetId="1" r:id="rId1"/>
+    <sheet name="РХБЗ" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="EmptyRows">ОВУ!$A$14</definedName>
-    <definedName name="RegisterDate">ОВУ!$A$5</definedName>
-    <definedName name="SoldierList">ОВУ!$A$13</definedName>
-    <definedName name="Заголовок">ОВУ!$A$2</definedName>
-    <definedName name="ИмяПодразделения">ОВУ!$A$3</definedName>
-    <definedName name="КВ">ОВУ!$A$6</definedName>
-    <definedName name="Подпись">ОВУ!$A$20</definedName>
-    <definedName name="Преподаватели">ОВУ!$A$7</definedName>
+    <definedName name="EmptyRows">РХБЗ!$A$14</definedName>
+    <definedName name="RegisterDate">РХБЗ!$A$5</definedName>
+    <definedName name="SoldierList">РХБЗ!$A$13</definedName>
+    <definedName name="Заголовок">РХБЗ!$A$2</definedName>
+    <definedName name="ИмяПодразделения">РХБЗ!$A$3</definedName>
+    <definedName name="КВ">РХБЗ!$A$6</definedName>
+    <definedName name="Подпись">РХБЗ!$A$20</definedName>
+    <definedName name="Преподаватели">РХБЗ!$A$7</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -326,6 +326,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -349,33 +376,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,55 +678,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
@@ -744,126 +744,126 @@
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="26"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="26"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="34"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="20" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="23" t="s">
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23" t="s">
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="4">
         <v>1</v>
       </c>
@@ -873,7 +873,7 @@
       <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="4">
         <v>1</v>
       </c>
@@ -883,9 +883,9 @@
       <c r="J11" s="4">
         <v>3</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
@@ -1040,31 +1040,24 @@
       <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A7:M7"/>
     <mergeCell ref="A20:M20"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:B11"/>
@@ -1077,6 +1070,13 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:K11"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A7:M7"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="257" scale="92" orientation="portrait" horizontalDpi="4294967295" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed print area range in some templates
</commit_message>
<xml_diff>
--- a/templates/ведомость_курсанты_РХБЗ.xlsx
+++ b/templates/ведомость_курсанты_РХБЗ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Pronko\prj\Grader\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YUKI\3_Вирусы\Pronko_2\prj\Grader\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,6 +22,7 @@
     <definedName name="Заголовок">РХБЗ!$A$2</definedName>
     <definedName name="ИмяПодразделения">РХБЗ!$A$3</definedName>
     <definedName name="КВ">РХБЗ!$A$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">РХБЗ!$A$1:$M$20</definedName>
     <definedName name="Подпись">РХБЗ!$A$20</definedName>
     <definedName name="Преподаватели">РХБЗ!$A$7</definedName>
   </definedNames>
@@ -327,6 +328,33 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -350,33 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,7 +666,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="A5" sqref="A5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -679,55 +680,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
     </row>
     <row r="2" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
@@ -745,126 +746,126 @@
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="34"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="26"/>
     </row>
     <row r="6" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="34"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="26"/>
     </row>
     <row r="7" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="34"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
     </row>
     <row r="8" spans="1:13" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="20" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="23" t="s">
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="32" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23" t="s">
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="23" t="s">
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="4">
         <v>1</v>
       </c>
@@ -874,7 +875,7 @@
       <c r="F11" s="4">
         <v>3</v>
       </c>
-      <c r="G11" s="25"/>
+      <c r="G11" s="34"/>
       <c r="H11" s="4">
         <v>1</v>
       </c>
@@ -884,9 +885,9 @@
       <c r="J11" s="4">
         <v>3</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
@@ -1041,31 +1042,24 @@
       <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A6:M6"/>
-    <mergeCell ref="A7:M7"/>
     <mergeCell ref="A20:M20"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B9:B11"/>
@@ -1078,6 +1072,13 @@
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:K11"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="A7:M7"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="257" scale="92" orientation="portrait" horizontalDpi="4294967295" verticalDpi="300" r:id="rId1"/>

</xml_diff>